<commit_message>
Complete join associations code. Started violin.
</commit_message>
<xml_diff>
--- a/Results/1_descriptiveTables.xlsx
+++ b/Results/1_descriptiveTables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
   <si>
     <t>N</t>
   </si>
@@ -22,97 +22,91 @@
     <t>age</t>
   </si>
   <si>
-    <t>48.7 ± 7.4</t>
-  </si>
-  <si>
-    <t>smoking</t>
-  </si>
-  <si>
-    <t>1767.7 ± 3643.2</t>
+    <t>48.9 (42.9-54.6)</t>
   </si>
   <si>
     <t>diet</t>
   </si>
   <si>
-    <t>24.9 ± 4.5</t>
+    <t>25.0 (22.0-28.0)</t>
   </si>
   <si>
     <t>alcohol</t>
   </si>
   <si>
-    <t>1.9 ± 2.0</t>
+    <t>1.5 (0.3-3.5)</t>
   </si>
   <si>
     <t>paeeTt</t>
   </si>
   <si>
-    <t>49.3 ± 19.9</t>
+    <t>46.9 (34.9-60.9)</t>
   </si>
   <si>
     <t>fatMass</t>
   </si>
   <si>
-    <t>27.5 ± 10.5</t>
+    <t>25.5 (20.1-32.8)</t>
   </si>
   <si>
     <t>fatFreeMass</t>
   </si>
   <si>
-    <t>41.5 ± 5.5</t>
+    <t>41.0 (37.7-44.6)</t>
   </si>
   <si>
     <t>insulin</t>
   </si>
   <si>
-    <t>43.1 ± 33.8</t>
+    <t>35.0 (24.6-51.0)</t>
   </si>
   <si>
     <t>leptin</t>
   </si>
   <si>
-    <t>23.3 ± 20.3</t>
+    <t>17.4 (9.4-30.6)</t>
   </si>
   <si>
     <t>nefa</t>
   </si>
   <si>
-    <t>372.4 ± 171.9</t>
+    <t>346.0 (244.5-476.0)</t>
   </si>
   <si>
     <t>ldl</t>
   </si>
   <si>
-    <t>3.3 ± 0.9</t>
+    <t>3.2 (2.7-3.8)</t>
   </si>
   <si>
     <t>adiponectin</t>
   </si>
   <si>
-    <t>8.8 ± 4.1</t>
+    <t>8.1 (5.9-11.0)</t>
   </si>
   <si>
     <t>crp</t>
   </si>
   <si>
-    <t>3.0 ± 5.2</t>
+    <t>1.5 (0.6-3.5)</t>
   </si>
   <si>
     <t>mbpdia</t>
   </si>
   <si>
-    <t>72.8 ± 9.9</t>
+    <t>72.0 (65.7-79.0)</t>
   </si>
   <si>
     <t>mbpsys</t>
   </si>
   <si>
-    <t>119.0 ± 15.6</t>
+    <t>116.7 (108.0-127.7)</t>
   </si>
   <si>
     <t>glucose0</t>
   </si>
   <si>
-    <t>4.7 ± 0.5</t>
+    <t>4.6 (4.4-4.9)</t>
   </si>
   <si>
     <t>ethnic: white</t>
@@ -193,6 +187,36 @@
     <t>0.0% (0)</t>
   </si>
   <si>
+    <t>smoke: Never smoked</t>
+  </si>
+  <si>
+    <t>56.1% (3513)</t>
+  </si>
+  <si>
+    <t>smoke: Ex smoker</t>
+  </si>
+  <si>
+    <t>32.0% (2001)</t>
+  </si>
+  <si>
+    <t>smoke: Current smoker</t>
+  </si>
+  <si>
+    <t>10.8% (674)</t>
+  </si>
+  <si>
+    <t>smoke: Missing/Unknown</t>
+  </si>
+  <si>
+    <t>1.2% (72)</t>
+  </si>
+  <si>
+    <t>smoke: Missing</t>
+  </si>
+  <si>
+    <t>0.0% (0)</t>
+  </si>
+  <si>
     <t>work_s: Sedentary</t>
   </si>
   <si>
@@ -343,97 +367,91 @@
     <t>age</t>
   </si>
   <si>
-    <t>48.6 ± 7.6</t>
-  </si>
-  <si>
-    <t>smoking</t>
-  </si>
-  <si>
-    <t>2602.7 ± 5099.5</t>
+    <t>48.8 (42.6-54.9)</t>
   </si>
   <si>
     <t>diet</t>
   </si>
   <si>
-    <t>22.9 ± 4.6</t>
+    <t>23.0 (20.0-26.0)</t>
   </si>
   <si>
     <t>alcohol</t>
   </si>
   <si>
-    <t>2.6 ± 2.1</t>
+    <t>1.5 (0.5-3.5)</t>
   </si>
   <si>
     <t>paeeTt</t>
   </si>
   <si>
-    <t>58.6 ± 23.3</t>
+    <t>56.2 (41.7-72.9)</t>
   </si>
   <si>
     <t>fatMass</t>
   </si>
   <si>
-    <t>25.6 ± 8.7</t>
+    <t>24.6 (19.8-30.1)</t>
   </si>
   <si>
     <t>fatFreeMass</t>
   </si>
   <si>
-    <t>57.5 ± 7.1</t>
+    <t>57.2 (52.7-61.8)</t>
   </si>
   <si>
     <t>insulin</t>
   </si>
   <si>
-    <t>53.8 ± 44.0</t>
+    <t>43.4 (29.3-65.4)</t>
   </si>
   <si>
     <t>leptin</t>
   </si>
   <si>
-    <t>7.6 ± 7.3</t>
+    <t>5.6 (3.0-9.6)</t>
   </si>
   <si>
     <t>nefa</t>
   </si>
   <si>
-    <t>306.0 ± 145.8</t>
+    <t>279.0 (200.0-383.0)</t>
   </si>
   <si>
     <t>ldl</t>
   </si>
   <si>
-    <t>3.5 ± 0.9</t>
+    <t>3.5 (2.9-4.1)</t>
   </si>
   <si>
     <t>adiponectin</t>
   </si>
   <si>
-    <t>5.2 ± 2.4</t>
+    <t>4.8 (3.5-6.4)</t>
   </si>
   <si>
     <t>crp</t>
   </si>
   <si>
-    <t>2.7 ± 5.6</t>
+    <t>1.4 (0.6-3.0)</t>
   </si>
   <si>
     <t>mbpdia</t>
   </si>
   <si>
-    <t>76.5 ± 10.1</t>
+    <t>76.0 (69.7-82.7)</t>
   </si>
   <si>
     <t>mbpsys</t>
   </si>
   <si>
-    <t>127.2 ± 14.0</t>
+    <t>125.7 (117.7-135.3)</t>
   </si>
   <si>
     <t>glucose0</t>
   </si>
   <si>
-    <t>5.0 ± 0.7</t>
+    <t>4.9 (4.6-5.2)</t>
   </si>
   <si>
     <t>ethnic: white</t>
@@ -509,6 +527,36 @@
   </si>
   <si>
     <t>income: Missing</t>
+  </si>
+  <si>
+    <t>0.0% (0)</t>
+  </si>
+  <si>
+    <t>smoke: Never smoked</t>
+  </si>
+  <si>
+    <t>51.6% (2840)</t>
+  </si>
+  <si>
+    <t>smoke: Ex smoker</t>
+  </si>
+  <si>
+    <t>34.0% (1870)</t>
+  </si>
+  <si>
+    <t>smoke: Current smoker</t>
+  </si>
+  <si>
+    <t>13.3% (733)</t>
+  </si>
+  <si>
+    <t>smoke: Missing/Unknown</t>
+  </si>
+  <si>
+    <t>1.1% (61)</t>
+  </si>
+  <si>
+    <t>smoke: Missing</t>
   </si>
   <si>
     <t>0.0% (0)</t>
@@ -705,7 +753,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B67"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -836,11 +884,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="18">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -860,11 +908,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -900,11 +948,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="28">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>48</v>
       </c>
     </row>
@@ -940,11 +988,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="s">
+    <row r="34">
+      <c r="A34" t="s">
         <v>57</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>58</v>
       </c>
     </row>
@@ -980,11 +1028,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="s">
+    <row r="40">
+      <c r="A40" t="s">
         <v>67</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1020,27 +1068,27 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" t="s">
-        <v>78</v>
-      </c>
-    </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
         <v>81</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1076,11 +1124,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="s">
+    <row r="54">
+      <c r="A54" t="s">
         <v>91</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1108,11 +1156,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s">
+    <row r="58">
+      <c r="A58" t="s">
         <v>99</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B58" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1138,6 +1186,38 @@
       </c>
       <c r="B62" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1146,12 +1226,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B68"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B1">
         <v>5504</v>
@@ -1159,434 +1239,466 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" t="s">
-        <v>139</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21" t="s">
-        <v>145</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>164</v>
-      </c>
-      <c r="B33" t="s">
-        <v>165</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>184</v>
+      </c>
+      <c r="B41" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B44" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>186</v>
-      </c>
-      <c r="B46" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B51" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" t="s">
-        <v>201</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>208</v>
+      </c>
+      <c r="B55" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B56" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B57" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B58" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>208</v>
-      </c>
-      <c r="B60" t="s">
-        <v>209</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B61" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>215</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>226</v>
+      </c>
+      <c r="B66" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>228</v>
+      </c>
+      <c r="B67" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>230</v>
+      </c>
+      <c r="B68" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 3_violinPlots code. Minor edits to other code. Ran code from 1 through 3, with updated results.
</commit_message>
<xml_diff>
--- a/Results/1_descriptiveTables.xlsx
+++ b/Results/1_descriptiveTables.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="female" sheetId="1" r:id="rId2"/>
-    <sheet name="male" sheetId="2" r:id="rId4"/>
+    <sheet name="Women" sheetId="1" r:id="rId2"/>
+    <sheet name="Men" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>

</xml_diff>